<commit_message>
peerji - aug -28
</commit_message>
<xml_diff>
--- a/TestData/logins.xlsx
+++ b/TestData/logins.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41E174E-C1E4-6842-8202-1074D42E3DB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C12DE0AC-5613-7A41-8D47-CD3D24B839F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-660" windowWidth="38400" windowHeight="19540" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-660" windowWidth="38400" windowHeight="19540" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -146,7 +146,7 @@
     <t>H1772773774775776778</t>
   </si>
   <si>
-    <t>testeq7867+1@gmail.com</t>
+    <t>sarikaqa7+nr2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -754,7 +754,7 @@
     <hyperlink ref="A3" r:id="rId1" xr:uid="{1C94BA48-9649-1746-9DE6-55F8B3DA6B11}"/>
     <hyperlink ref="A5" r:id="rId2" xr:uid="{14FF7464-C1D3-BF41-BC72-83E0FD1CB997}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{8A288E0E-7F0E-0941-BD31-72C41B6F7069}"/>
-    <hyperlink ref="A2" r:id="rId4" xr:uid="{510A385A-93F7-D64C-B9AF-C0146D5D4D24}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{027109FE-318F-A54F-AE5C-7BA20A10C634}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A06E5BC-F834-5B48-98D0-3C57F0FF5E9E}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Peerji - Oct 07
</commit_message>
<xml_diff>
--- a/TestData/logins.xlsx
+++ b/TestData/logins.xlsx
@@ -3,26 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10913"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C605ABB-134B-DB48-AF20-D47053456D1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A1F989-EA0B-3E4E-8088-B5FD9FDBD877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="18740" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="18740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
     <sheet name="UAT" sheetId="2" r:id="rId2"/>
     <sheet name="Prod" sheetId="3" r:id="rId3"/>
     <sheet name="EQCare" sheetId="4" r:id="rId4"/>
-    <sheet name="Clinic" sheetId="5" r:id="rId5"/>
-    <sheet name="Users" sheetId="6" r:id="rId6"/>
-    <sheet name="Practitest" sheetId="8" r:id="rId7"/>
-    <sheet name="Nova" sheetId="7" r:id="rId8"/>
+    <sheet name="Login" sheetId="9" r:id="rId5"/>
+    <sheet name="Clinic" sheetId="5" r:id="rId6"/>
+    <sheet name="Users" sheetId="6" r:id="rId7"/>
+    <sheet name="Practitest" sheetId="8" r:id="rId8"/>
+    <sheet name="Nova" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>Admin</t>
   </si>
@@ -151,13 +152,43 @@
   </si>
   <si>
     <t>Test Cases</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Account Edit Personal Information</t>
+  </si>
+  <si>
+    <t>Account Edit Account Information</t>
+  </si>
+  <si>
+    <t>29754452</t>
+  </si>
+  <si>
+    <t>Account Upload Profile Pic</t>
+  </si>
+  <si>
+    <t>Account Uplaod Govt Id</t>
+  </si>
+  <si>
+    <t>Family Tab visible</t>
+  </si>
+  <si>
+    <t>Add Child</t>
+  </si>
+  <si>
+    <t>Delete Child</t>
+  </si>
+  <si>
+    <t>sarikaqa7+j1@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +240,40 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -218,7 +283,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -241,12 +306,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -260,7 +338,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -692,7 +778,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -767,6 +853,41 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D04AB40-EB56-A14B-8FB4-388B0BBF584C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{452FF465-3101-B947-BD8C-AC29CFCB2980}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -808,7 +929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A06E5BC-F834-5B48-98D0-3C57F0FF5E9E}">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -941,38 +1062,119 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAF7634-3827-E648-9486-6E72DB2D1D0A}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="69.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>28919642</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
+    <row r="2" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>29754173</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>29754390</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>29754391</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>29754448</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>29754451</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>29840573</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="23" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>29840574</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF550E68-59AC-7C47-9024-4BAF9464D212}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>